<commit_message>
added table from 23.10.2023
</commit_message>
<xml_diff>
--- a/Year 1 - 2023-2024/Modul 1/Excel/23.10.2023 HW/Комплексно задание - Обменно бюро (1).xlsx
+++ b/Year 1 - 2023-2024/Modul 1/Excel/23.10.2023 HW/Комплексно задание - Обменно бюро (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Github Repos\IT\Year 1 - 2023-2024\Modul 1\Excel\23.10.2023 HW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\IT\Year 1 - 2023-2024\Modul 1\Excel\23.10.2023 HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6272F122-BAE9-4D77-AF4E-A2928F85DEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB723D61-C5D4-472E-8A23-BBB46211834B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Бордера" sheetId="4" r:id="rId1"/>
@@ -116,16 +116,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;лв.&quot;_-;\-* #,##0.00\ &quot;лв.&quot;_-;_-* &quot;-&quot;??\ &quot;лв.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="167" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$CHF-100C]_-;\-* #,##0.00\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
+  <numFmts count="7">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;лв.&quot;_-;\-* #,##0.00\ &quot;лв.&quot;_-;_-* &quot;-&quot;??\ &quot;лв.&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="168" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.00\ [$CHF-100C]_-;\-* #,##0.00\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0.0000\ &quot;лв.&quot;_-;\-* #,##0.0000\ &quot;лв.&quot;_-;_-* &quot;-&quot;??\ &quot;лв.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="[$£-809]#,##0.00"/>
-    <numFmt numFmtId="174" formatCode="#,##0.00\ _л_в_."/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -200,24 +198,24 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -225,46 +223,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -548,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,21 +564,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="F1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="F1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -634,7 +635,7 @@
       <c r="G4" s="15">
         <v>1000</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="27">
         <f>VLOOKUP(F4,Valuti,4,FALSE)*G4</f>
         <v>1000</v>
       </c>
@@ -674,19 +675,19 @@
       <c r="G5" s="18">
         <v>500</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="27">
         <f>VLOOKUP(F5,Valuti,4,FALSE)*G5</f>
         <v>977.91499999999996</v>
       </c>
-      <c r="I5" s="15">
-        <f>IF(F5="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F5,B$13:B$19,"Купува"))</f>
-        <v>97.25</v>
-      </c>
-      <c r="J5" s="16">
-        <f>IF(F5="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F5,B$13:B$19,"Продава"))</f>
-        <v>372.4</v>
-      </c>
-      <c r="K5" s="18">
+      <c r="I5" s="29">
+        <f>IF(F5="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F5,B$13:B$19,"Купува"))</f>
+        <v>50</v>
+      </c>
+      <c r="J5" s="30">
+        <f>IF(F5="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F5,B$13:B$19,"Продава"))</f>
+        <v>190</v>
+      </c>
+      <c r="K5" s="31">
         <f>SUMIFS(D$13:D$19,C$13:C$19,F5,B$13:B$19,"Купува")-SUMIFS(D$13:D$19,C$13:C$19,F5,B$13:B$19,"Продава")+G5</f>
         <v>360</v>
       </c>
@@ -714,19 +715,19 @@
       <c r="G6" s="20">
         <v>800</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="27">
         <f>VLOOKUP(F6,Valuti,4,FALSE)*G6</f>
         <v>1335.4960000000001</v>
       </c>
-      <c r="I6" s="15">
-        <f>IF(F6="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F6,B$13:B$19,"Купува"))</f>
-        <v>494.82</v>
-      </c>
-      <c r="J6" s="16">
-        <f>IF(F6="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F6,B$13:B$19,"Продава"))</f>
+      <c r="I6" s="29">
+        <f>IF(F6="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F6,B$13:B$19,"Купува"))</f>
+        <v>300</v>
+      </c>
+      <c r="J6" s="30">
+        <f>IF(F6="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F6,B$13:B$19,"Продава"))</f>
         <v>0</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="32">
         <f t="shared" ref="K6:K8" si="0">SUMIFS(D$13:D$19,C$13:C$19,F6,B$13:B$19,"Купува")-SUMIFS(D$13:D$19,C$13:C$19,F6,B$13:B$19,"Продава")+G6</f>
         <v>1100</v>
       </c>
@@ -754,19 +755,19 @@
       <c r="G7" s="21">
         <v>600</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="27">
         <f>VLOOKUP(F7,Valuti,4,FALSE)*G7</f>
         <v>1320.6120000000001</v>
       </c>
-      <c r="I7" s="15">
-        <f>IF(F7="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F7,B$13:B$19,"Купува"))</f>
+      <c r="I7" s="29">
+        <f>IF(F7="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F7,B$13:B$19,"Купува"))</f>
         <v>0</v>
       </c>
-      <c r="J7" s="16">
-        <f>IF(F7="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F7,B$13:B$19,"Продава"))</f>
-        <v>560.00000000000011</v>
-      </c>
-      <c r="K7" s="30">
+      <c r="J7" s="30">
+        <f>IF(F7="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F7,B$13:B$19,"Продава"))</f>
+        <v>250</v>
+      </c>
+      <c r="K7" s="31">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
@@ -794,17 +795,17 @@
       <c r="G8" s="22">
         <v>700</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <f>VLOOKUP(F8,Valuti,4,FALSE)*G8</f>
         <v>1178.6179999999999</v>
       </c>
-      <c r="I8" s="15">
-        <f>IF(F8="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F8,B$13:B$19,"Купува"))</f>
-        <v>82.62</v>
-      </c>
-      <c r="J8" s="16">
-        <f>IF(F8="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(Стойност_в_лв.,C$13:C$19,F8,B$13:B$19,"Продава"))</f>
-        <v>429.42500000000001</v>
+      <c r="I8" s="29">
+        <f>IF(F8="BGN",SUMIF(B$13:B$19,"Продава",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F8,B$13:B$19,"Купува"))</f>
+        <v>50</v>
+      </c>
+      <c r="J8" s="30">
+        <f>IF(F8="BGN",SUMIF(B$13:B$19,"Купува",Стойност_в_лв.),SUMIFS(D$13:D$19,C$13:C$19,F8,B$13:B$19,"Продава"))</f>
+        <v>250</v>
       </c>
       <c r="K8" s="31">
         <f t="shared" si="0"/>
@@ -826,13 +827,13 @@
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
       <c r="G10" s="5" t="s">
         <v>15</v>
       </c>
@@ -872,8 +873,8 @@
       <c r="D13" s="24">
         <v>50</v>
       </c>
-      <c r="E13" s="27">
-        <f>VLOOKUP(C13,Valuti,MATCH(B13,Vidove,0)+1,FALSE)*D13</f>
+      <c r="E13" s="26">
+        <f t="shared" ref="E13:E19" si="1">VLOOKUP(C13,Valuti,MATCH(B13,Vidove,0)+1,FALSE)*D13</f>
         <v>97.25</v>
       </c>
     </row>
@@ -890,8 +891,8 @@
       <c r="D14" s="25">
         <v>150</v>
       </c>
-      <c r="E14" s="27">
-        <f>VLOOKUP(C14,Valuti,MATCH(B14,Vidove,0)+1,FALSE)*D14</f>
+      <c r="E14" s="26">
+        <f t="shared" si="1"/>
         <v>336.00000000000006</v>
       </c>
     </row>
@@ -908,8 +909,8 @@
       <c r="D15" s="24">
         <v>50</v>
       </c>
-      <c r="E15" s="27">
-        <f>VLOOKUP(C15,Valuti,MATCH(B15,Vidove,0)+1,FALSE)*D15</f>
+      <c r="E15" s="26">
+        <f t="shared" si="1"/>
         <v>82.62</v>
       </c>
     </row>
@@ -926,8 +927,8 @@
       <c r="D16" s="25">
         <v>300</v>
       </c>
-      <c r="E16" s="27">
-        <f>VLOOKUP(C16,Valuti,MATCH(B16,Vidove,0)+1,FALSE)*D16</f>
+      <c r="E16" s="26">
+        <f t="shared" si="1"/>
         <v>494.82</v>
       </c>
     </row>
@@ -944,8 +945,8 @@
       <c r="D17" s="24">
         <v>250</v>
       </c>
-      <c r="E17" s="27">
-        <f>VLOOKUP(C17,Valuti,MATCH(B17,Vidove,0)+1,FALSE)*D17</f>
+      <c r="E17" s="26">
+        <f t="shared" si="1"/>
         <v>429.42500000000001</v>
       </c>
     </row>
@@ -962,8 +963,8 @@
       <c r="D18" s="25">
         <v>190</v>
       </c>
-      <c r="E18" s="27">
-        <f>VLOOKUP(C18,Valuti,MATCH(B18,Vidove,0)+1,FALSE)*D18</f>
+      <c r="E18" s="26">
+        <f t="shared" si="1"/>
         <v>372.4</v>
       </c>
     </row>
@@ -980,8 +981,8 @@
       <c r="D19" s="24">
         <v>100</v>
       </c>
-      <c r="E19" s="27">
-        <f>VLOOKUP(C19,Valuti,MATCH(B19,Vidove,0)+1,FALSE)*D19</f>
+      <c r="E19" s="26">
+        <f t="shared" si="1"/>
         <v>224.00000000000003</v>
       </c>
     </row>

</xml_diff>